<commit_message>
Cambios casi finalizados, falta un pdf
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p31/P31_UO277876.xlsx
+++ b/src/main/java/algestudiante/p31/P31_UO277876.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p31\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8AF413-F7B0-4225-A58E-05E7D6414932}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B8331A-10C1-433F-907A-42CF15E8170F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
   <sheets>
     <sheet name="División" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>nVeces</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>O(n^2)</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -382,9 +385,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -6800,8 +6800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50AC779-C55D-4822-8A6D-58AA05F2A758}">
   <dimension ref="A2:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6816,10 +6816,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -6831,10 +6831,10 @@
       <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="14" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -6846,28 +6846,28 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>1</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <f>43/N3</f>
         <v>4.3000000000000001E-8</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <f>72/N3</f>
         <v>7.1999999999999996E-8</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="20">
         <f>136/N3</f>
         <v>1.36E-7</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="6" t="s">
@@ -6879,24 +6879,24 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="24">
         <v>2</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <f>2277/N3</f>
         <v>2.277E-6</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <f>9678/N3</f>
         <v>9.6779999999999995E-6</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="20">
         <f>23167/N3</f>
         <v>2.3167E-5</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="14"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="15"/>
       <c r="J4" s="8" t="s">
         <v>3</v>
       </c>
@@ -6906,70 +6906,70 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="24">
         <v>4</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <f>6026/N3</f>
         <v>6.0260000000000004E-6</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <f>12304/N3</f>
         <v>1.2303999999999999E-5</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <f>32322/N3</f>
         <v>3.2322E-5</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="14"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="15"/>
       <c r="N5" s="2">
         <v>10000000</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="24">
         <v>8</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <f>9023/N3</f>
         <v>9.0229999999999998E-6</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <f>43960/N3</f>
         <v>4.3959999999999999E-5</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <f>111959/N3</f>
         <v>1.11959E-4</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="14"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="15"/>
       <c r="N6" s="2">
         <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="24">
         <v>16</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="20">
         <f>15973/N3</f>
         <v>1.5973000000000001E-5</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <f>56325/N3</f>
         <v>5.6325E-5</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <f>14747/N4</f>
         <v>1.4747E-4</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="14" t="s">
+      <c r="F7" s="32"/>
+      <c r="G7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="N7" s="3">
@@ -6977,434 +6977,434 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="24">
         <v>32</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <f>26636/N3</f>
         <v>2.6636E-5</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <f>187266/N3</f>
         <v>1.8726600000000001E-4</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <f>48716/N4</f>
         <v>4.8715999999999999E-4</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="15"/>
       <c r="N8" s="2">
         <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="24">
         <v>64</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="20">
         <f>44220/N3</f>
         <v>4.422E-5</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <f>22697/N4</f>
         <v>2.2697E-4</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="20">
         <f>60786/N4</f>
         <v>6.0786E-4</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="N9" s="18">
+      <c r="G9" s="15"/>
+      <c r="N9" s="17">
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="24">
         <v>128</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="20">
         <f>90625/N3</f>
         <v>9.0624999999999994E-5</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <f>74843/N4</f>
         <v>7.4843000000000002E-4</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <f>191166/N4</f>
         <v>1.9116599999999999E-3</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="14"/>
-      <c r="N10" s="18">
+      <c r="F10" s="32"/>
+      <c r="G10" s="15"/>
+      <c r="N10" s="17">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="25">
+      <c r="B11" s="24">
         <v>256</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="20">
         <f>163451/N3</f>
         <v>1.63451E-4</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <f>93557/N4</f>
         <v>9.3557000000000004E-4</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="20">
         <f>24442/N5</f>
         <v>2.4442000000000001E-3</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="17">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="24">
         <v>512</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <f>34550/N4</f>
         <v>3.455E-4</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <f>75724/N5</f>
         <v>7.5724E-3</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <f>77121/N5</f>
         <v>7.7121000000000004E-3</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="N12" s="18">
+      <c r="G12" s="15"/>
+      <c r="N12" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="24">
         <v>1024</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <f>65558/N4</f>
         <v>6.5558000000000001E-4</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <f>85998/N5</f>
         <v>8.5997999999999995E-3</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="20">
         <f>99007/N5</f>
         <v>9.9007000000000001E-3</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="14"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="25">
+      <c r="B14" s="24">
         <v>2048</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="20">
         <f>127283/N4</f>
         <v>1.27283E-3</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <f>30221/N6</f>
         <v>3.0221000000000001E-2</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="20">
         <f>31795/N6</f>
         <v>3.1794999999999997E-2</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="24">
         <v>4096</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <f>26789/N5</f>
         <v>2.6789000000000001E-3</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="20">
         <f>50245/N6</f>
         <v>5.0244999999999998E-2</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="20">
         <f>39445/N6</f>
         <v>3.9445000000000001E-2</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="14"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="24">
         <v>8192</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="20">
         <f>46140/N5</f>
         <v>4.614E-3</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="20">
         <f>127559/N6</f>
         <v>0.12755900000000001</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <f>124094/N6</f>
         <v>0.124094</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="14"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="25">
+      <c r="B17" s="24">
         <v>16384</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="20">
         <f>93066/N5</f>
         <v>9.3065999999999999E-3</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="20">
         <f>20120/N7</f>
         <v>0.20119999999999999</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="20">
         <f>15563/N7</f>
         <v>0.15562999999999999</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="25">
+      <c r="B18" s="24">
         <v>32768</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="20">
         <f>198417/N5</f>
         <v>1.98417E-2</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="20">
         <f>50916/N7</f>
         <v>0.50915999999999995</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="20">
         <f>50015/N7</f>
         <v>0.50014999999999998</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="14"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="24">
         <v>65536</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="20">
         <f>39013/N6</f>
         <v>3.9012999999999999E-2</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="20">
         <f>88990/N7</f>
         <v>0.88990000000000002</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="20">
         <f>62243/N7</f>
         <v>0.62243000000000004</v>
       </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="14"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="25">
+      <c r="B20" s="24">
         <v>131072</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="20">
         <f>89397/N6</f>
         <v>8.9397000000000004E-2</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="20">
         <f>216177/N7</f>
         <v>2.1617700000000002</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="20">
         <f>199343/N7</f>
         <v>1.99343</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="14"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="25">
+      <c r="B21" s="24">
         <v>262144</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <f>151148/N6</f>
         <v>0.151148</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <f>40482/N8</f>
         <v>4.0481999999999996</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="20">
         <f>24759/N8</f>
         <v>2.4759000000000002</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="26">
+      <c r="B22" s="25">
         <v>524288</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <f>64521/N7</f>
         <v>0.64520999999999995</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="20">
         <f>100725/N8</f>
         <v>10.0725</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="20">
         <f>78658/N8</f>
         <v>7.8658000000000001</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="14"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="26">
+      <c r="B23" s="25">
         <v>1048576</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="20">
         <f>128562/N7</f>
         <v>1.28562</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="20">
         <f>17652/N9</f>
         <v>17.652000000000001</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="20">
         <f>99711/N8</f>
         <v>9.9710999999999999</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="25">
         <v>2097152</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="20">
         <f>12126/N8</f>
         <v>1.2125999999999999</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="20">
         <f>42898/N9</f>
         <v>42.898000000000003</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="20">
         <f>32111/N9</f>
         <v>32.110999999999997</v>
       </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="14" t="s">
+      <c r="F24" s="32"/>
+      <c r="G24" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" s="26">
+      <c r="B25" s="25">
         <v>4194304</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="20">
         <f>24027/N8</f>
         <v>2.4026999999999998</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="20">
         <f>74670/N9</f>
         <v>74.67</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="20">
         <f>40085/N9</f>
         <v>40.085000000000001</v>
       </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="14"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="28">
+      <c r="A26" s="16"/>
+      <c r="B26" s="27">
         <v>8388608</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="21">
         <f>48531/N8</f>
         <v>4.8531000000000004</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="21">
         <f>181709/N9</f>
         <v>181.709</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="21">
         <f>126504/N9</f>
         <v>126.504</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="9"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="33" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7417,10 +7417,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B473716-F3A2-49BD-996D-A970964813E6}">
-  <dimension ref="A2:N19"/>
+  <dimension ref="A2:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7434,10 +7434,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -7449,10 +7449,10 @@
       <c r="E2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -7464,28 +7464,28 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>1</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="26">
         <f>90/N3</f>
         <v>8.9999999999999999E-8</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="26">
         <f>72/N5</f>
         <v>7.1999999999999997E-6</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="26">
         <f>89/N3</f>
         <v>8.9000000000000003E-8</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="6" t="s">
@@ -7497,24 +7497,24 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="23">
+      <c r="A4" s="15"/>
+      <c r="B4" s="22">
         <v>2</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <f>5116/N3</f>
         <v>5.1159999999999998E-6</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <f>196/N5</f>
         <v>1.9599999999999999E-5</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <f>23391/N3</f>
         <v>2.3391E-5</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="13"/>
       <c r="J4" s="8" t="s">
         <v>3</v>
       </c>
@@ -7524,47 +7524,47 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="23">
+      <c r="A5" s="15"/>
+      <c r="B5" s="22">
         <v>4</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <f>12503/N3</f>
         <v>1.2503E-5</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <f>345/N5</f>
         <v>3.4499999999999998E-5</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <f>131145/N3</f>
         <v>1.3114499999999999E-4</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="13"/>
       <c r="N5" s="2">
         <v>10000000</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="23">
+      <c r="A6" s="15"/>
+      <c r="B6" s="22">
         <v>8</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <f>28139/N3</f>
         <v>2.8138999999999999E-5</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <f>980/N5</f>
         <v>9.7999999999999997E-5</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <f>164955/N4</f>
         <v>1.6495500000000001E-3</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="14" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="13" t="s">
         <v>18</v>
       </c>
       <c r="N6" s="2">
@@ -7572,24 +7572,24 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="23">
+      <c r="A7" s="15"/>
+      <c r="B7" s="22">
         <v>16</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <f>56745/N3</f>
         <v>5.6745E-5</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="26">
         <f>2969/N5</f>
         <v>2.9690000000000001E-4</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <f>377930/N6</f>
         <v>0.37792999999999999</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="14" t="s">
+      <c r="F7" s="15"/>
+      <c r="G7" s="13" t="s">
         <v>32</v>
       </c>
       <c r="N7" s="3">
@@ -7597,24 +7597,24 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="23">
+      <c r="A8" s="15"/>
+      <c r="B8" s="22">
         <v>32</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="26">
         <f>118253/N3</f>
         <v>1.1825299999999999E-4</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="26">
         <f>14534/N5</f>
         <v>1.4534000000000001E-3</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <f>142971/N11</f>
         <v>14297.1</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="14" t="s">
+      <c r="F8" s="15"/>
+      <c r="G8" s="13" t="s">
         <v>33</v>
       </c>
       <c r="N8" s="2">
@@ -7622,216 +7622,221 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>64</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="26">
         <f>13858/N4</f>
         <v>1.3857999999999999E-4</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <f>62896/N5</f>
         <v>6.2896000000000002E-3</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="14"/>
-      <c r="N9" s="18">
+      <c r="E9" s="26"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="13"/>
+      <c r="N9" s="17">
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="23">
+      <c r="A10" s="15"/>
+      <c r="B10" s="22">
         <v>128</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="26">
         <f>26158/N4</f>
         <v>2.6158000000000003E-4</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="26">
         <f>227592/N5</f>
         <v>2.27592E-2</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="14"/>
-      <c r="N10" s="18">
+      <c r="E10" s="26"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="13"/>
+      <c r="N10" s="17">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="23">
+      <c r="A11" s="15"/>
+      <c r="B11" s="22">
         <v>256</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="26">
         <f>56185/N4</f>
         <v>5.6185000000000002E-4</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="26">
         <f>81768/N6</f>
         <v>8.1767999999999993E-2</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="16" t="s">
+      <c r="E11" s="26"/>
+      <c r="F11" s="15" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="N11" s="18">
+      <c r="N11" s="17">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="33"/>
-      <c r="B12" s="23">
+      <c r="A12" s="32"/>
+      <c r="B12" s="22">
         <v>512</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="26">
         <f>106063/N4</f>
         <v>1.0606299999999999E-3</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="26">
         <f>305027/N6</f>
         <v>0.30502699999999999</v>
       </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="7"/>
-      <c r="N12" s="18">
+      <c r="N12" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="22">
         <v>1024</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="26">
         <f>42931/N5</f>
         <v>4.2931000000000002E-3</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="26">
         <f>152492/N7</f>
         <v>1.5249200000000001</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="16" t="s">
+      <c r="E13" s="26"/>
+      <c r="F13" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="33"/>
-      <c r="B14" s="23">
+      <c r="A14" s="32"/>
+      <c r="B14" s="22">
         <v>2048</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="26">
         <f>94697/N5</f>
         <v>9.4696999999999993E-3</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="26">
         <f>45935/N8</f>
         <v>4.5934999999999997</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="16" t="s">
+      <c r="E14" s="26"/>
+      <c r="F14" s="15" t="s">
         <v>29</v>
       </c>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="22">
         <v>4098</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="26">
         <f>19399/N6</f>
         <v>1.9399E-2</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="26">
         <f>180036/N8</f>
         <v>18.003599999999999</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="16"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
-      <c r="B16" s="23">
+      <c r="A16" s="32"/>
+      <c r="B16" s="22">
         <v>8192</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="26">
         <f>39403/N6</f>
         <v>3.9403000000000001E-2</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="26">
         <f>76408/N9</f>
         <v>76.408000000000001</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="26"/>
+      <c r="F16" s="15" t="s">
         <v>30</v>
       </c>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <v>16384</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="26">
         <f>79860/N6</f>
         <v>7.986E-2</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="26">
         <f>304687/N9</f>
         <v>304.68700000000001</v>
       </c>
-      <c r="E17" s="27"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="3"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="30">
+      <c r="A18" s="16"/>
+      <c r="B18" s="29">
         <v>32768</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="28">
         <f>161291/N6</f>
         <v>0.16129099999999999</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="28">
         <f>40918/N10</f>
         <v>409.18</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="31" t="s">
+      <c r="E18" s="28"/>
+      <c r="F18" s="30" t="s">
         <v>31</v>
       </c>
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="33" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K39" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>